<commit_message>
update test suite doc
</commit_message>
<xml_diff>
--- a/doc/SfcTestSuite.xlsx
+++ b/doc/SfcTestSuite.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
     <sheet name="Procedure" sheetId="1" r:id="rId2"/>
+    <sheet name="Operation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Spec</t>
   </si>
@@ -36,9 +37,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Procedure sets</t>
-  </si>
-  <si>
     <t>This document contains many pages (worksheets); pages generally correspond to specifications for a particular SFC step type, but may also refer to programmatic apis, or whatever makes sense</t>
   </si>
   <si>
@@ -66,9 +64,6 @@
     <t>The available methods are: startTest, assertTrue, failTest, passTest, and reportTests. startTest is called from the Run Suite button action script</t>
   </si>
   <si>
-    <t>In your top-level chart, add an onStop method calling passTest, and onAbort and onCancel methods calling failTest (see the Trivial test for examples)</t>
-  </si>
-  <si>
     <t>specifications are generally tested by calling "assertTrue" in Action Step onStart scripts</t>
   </si>
   <si>
@@ -115,6 +110,24 @@
   </si>
   <si>
     <t>these might be automated tests started with startTest but minus the canned user response</t>
+  </si>
+  <si>
+    <t>MessageQueue</t>
+  </si>
+  <si>
+    <t>messageQueue property sets current message queue</t>
+  </si>
+  <si>
+    <t>implementation: value held in top chart scope</t>
+  </si>
+  <si>
+    <t>(optional) messageQueue property sets current message queue</t>
+  </si>
+  <si>
+    <t>IN ALL CHARTS add onAbort and onCancel methods calling failTest (see the Trivial test for examples)</t>
+  </si>
+  <si>
+    <t>in the top level chart only, add an onStop method calling passTest</t>
   </si>
 </sst>
 </file>
@@ -432,142 +445,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>21</v>
+      <c r="B27" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>14</v>
+      <c r="C28" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -580,12 +598,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="49.28515625" customWidth="1"/>
     <col min="2" max="2" width="46.28515625" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" customWidth="1"/>
   </cols>
@@ -603,7 +621,54 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enhancements and bug fixes for Review Data step
</commit_message>
<xml_diff>
--- a/doc/SfcTestSuite.xlsx
+++ b/doc/SfcTestSuite.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="8790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
-    <sheet name="Procedure" sheetId="1" r:id="rId2"/>
-    <sheet name="Operation" sheetId="3" r:id="rId3"/>
+    <sheet name="Review Data" sheetId="4" r:id="rId2"/>
+    <sheet name="Procedure" sheetId="1" r:id="rId3"/>
+    <sheet name="Operation" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Spec</t>
   </si>
@@ -128,6 +129,54 @@
   </si>
   <si>
     <t>in the top level chart only, add an onStop method calling passTest</t>
+  </si>
+  <si>
+    <t>Manual:</t>
+  </si>
+  <si>
+    <t>header property shown as window title</t>
+  </si>
+  <si>
+    <t>button property results in "top" button on ctrl panel</t>
+  </si>
+  <si>
+    <t>window property can name alternate window</t>
+  </si>
+  <si>
+    <t>omit posting method??</t>
+  </si>
+  <si>
+    <t>button response saved in recipe data key</t>
+  </si>
+  <si>
+    <t>gui position/scale control dialog location/size</t>
+  </si>
+  <si>
+    <t>configuration stored @ configuration key</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>?? Don't see prompt show up in screen shot</t>
+  </si>
+  <si>
+    <t>units conversion between recipe data units and configured "view" units</t>
+  </si>
+  <si>
+    <t>in a string valued recipe data editable with s88Set</t>
+  </si>
+  <si>
+    <t>posting method populates window</t>
+  </si>
+  <si>
+    <t>specify default, takes same params</t>
+  </si>
+  <si>
+    <t>?? Omit display mode, make secondary data a tab in same window</t>
+  </si>
+  <si>
+    <t>values read from recipe data (value with units)</t>
   </si>
 </sst>
 </file>
@@ -447,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -594,6 +643,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -635,7 +789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>